<commit_message>
added cases for Login with null or invalid data
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADCA94F-5110-4B14-9071-71B45A9D5D4B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44059C42-1454-4667-9D45-F8245AE58C44}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Email</t>
   </si>
@@ -41,6 +41,43 @@
   </si>
   <si>
     <t>Valid user</t>
+  </si>
+  <si>
+    <t>Jasmine</t>
+  </si>
+  <si>
+    <t>Valid email &amp; invalid password</t>
+  </si>
+  <si>
+    <t>123@gmail.com</t>
+  </si>
+  <si>
+    <t>Null email &amp; null password</t>
+  </si>
+  <si>
+    <t>Valid email &amp; null password</t>
+  </si>
+  <si>
+    <t>Null email &amp; password</t>
+  </si>
+  <si>
+    <t>Invalid email &amp; password</t>
+  </si>
+  <si>
+    <t>Invalid email &amp; null password</t>
+  </si>
+  <si>
+    <t>jasmine.liu012005@gmail.com</t>
+  </si>
+  <si>
+    <t>345@mail.com</t>
+  </si>
+  <si>
+    <t>123@mail</t>
+  </si>
+  <si>
+    <t>You've subscribed to a GrabOne newsletter, but you haven't registered. 
+Please register here.</t>
   </si>
 </sst>
 </file>
@@ -110,7 +147,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -124,8 +161,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -407,17 +448,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
     <col min="6" max="7" width="10.42578125" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
@@ -483,10 +524,14 @@
       <c r="P2" s="4"/>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="4"/>
@@ -501,10 +546,18 @@
       <c r="P3" s="4"/>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -519,10 +572,16 @@
       <c r="P4" s="1"/>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -537,10 +596,16 @@
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="1:16">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -555,10 +620,18 @@
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="6"/>
       <c r="G7" s="2"/>
@@ -573,17 +646,37 @@
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="1:16">
-      <c r="B8" s="7"/>
+      <c r="A8" s="8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+      <c r="D8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="10" spans="1:16" ht="45">
+      <c r="B10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{BBE11251-54E7-4526-BDBE-0BA98542BA64}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{69F9B155-7A46-4421-B635-EC716CD68FF3}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{AAFAB02D-E96A-40A5-B220-127AFE904A9A}"/>
+    <hyperlink ref="B7" r:id="rId4" xr:uid="{BF1249C2-F10F-4D58-8290-F092F39BCD56}"/>
+    <hyperlink ref="B8" r:id="rId5" xr:uid="{5839BE08-6268-4CEA-9D17-660FDCD90F07}"/>
+    <hyperlink ref="B10" r:id="rId6" xr:uid="{BD7186B7-11C1-4C2C-986B-AD004F33B746}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>